<commit_message>
Correction of Simplex Method
</commit_message>
<xml_diff>
--- a/Python/ONB.xlsx
+++ b/Python/ONB.xlsx
@@ -469,7 +469,7 @@
   <dimension ref="A1:X2375"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1145,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -1160,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>

</xml_diff>